<commit_message>
new bill of materials with orders for 50 boards based on what we have in stock already
</commit_message>
<xml_diff>
--- a/v0.2-bom.xlsx
+++ b/v0.2-bom.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeannettecirce/Desktop/rcc-pico-shield/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E762CE-B141-2F43-8D8E-393FECFEC220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B27705-E7D6-AA46-AFF2-DA54393D0441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="27580" windowHeight="16940" xr2:uid="{7B30E689-66B9-5747-BDE2-2969221BC952}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="18520" windowHeight="17500" xr2:uid="{7B30E689-66B9-5747-BDE2-2969221BC952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="176">
   <si>
     <t>Source:</t>
   </si>
@@ -521,6 +521,48 @@
   </si>
   <si>
     <t>3147-B1911USD-20D000114U1930CT-ND</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>custom-components:DIOM5227X270N</t>
+  </si>
+  <si>
+    <t>SX32_R1_00001</t>
+  </si>
+  <si>
+    <t>30 Pcs 40 pin Breakable Pin Header 2.54mm Single Row Male Header Connector Kit PCB Pin Strip for Arduino</t>
+  </si>
+  <si>
+    <t>Female Headers</t>
+  </si>
+  <si>
+    <t>Multicolor Male Headers</t>
+  </si>
+  <si>
+    <t>Qunqi 60Pcs 40 Pin 2.54mm Single Row Straight Female PCB Header Connector Strip for Arduino Shield</t>
+  </si>
+  <si>
+    <t>SC0918</t>
+  </si>
+  <si>
+    <t>Male Headers</t>
+  </si>
+  <si>
+    <t>we have</t>
+  </si>
+  <si>
+    <t>need for 50 boards</t>
+  </si>
+  <si>
+    <t>need to buy</t>
+  </si>
+  <si>
+    <t>ordering</t>
   </si>
 </sst>
 </file>
@@ -530,7 +572,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -572,12 +614,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -601,22 +637,39 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -926,23 +979,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEC4177-0387-0E47-BF1F-F48A6F075E39}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="36.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="53" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" hidden="1" customWidth="1"/>
     <col min="7" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="37.1640625" customWidth="1"/>
-    <col min="15" max="16" width="10.83203125" style="6"/>
+    <col min="13" max="13" width="14.5" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
+    <col min="15" max="16" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +1015,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -978,7 +1033,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -996,7 +1051,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1069,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1032,7 +1087,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1046,7 +1101,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1061,8 +1116,20 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>172</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1076,7 +1143,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1114,7 +1181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1141,11 +1208,22 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="7" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <v>183</v>
+      </c>
+      <c r="O10" s="8">
+        <f>B10*50</f>
+        <v>100</v>
+      </c>
+      <c r="P10" s="8">
+        <f>O10-N10</f>
+        <v>-83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1172,11 +1250,22 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="7" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <v>184</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" ref="O11:O29" si="0">B11*50</f>
+        <v>100</v>
+      </c>
+      <c r="P11" s="8">
+        <f t="shared" ref="P11:P32" si="1">O11-N11</f>
+        <v>-84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -1203,11 +1292,22 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <v>184</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="P12" s="8">
+        <f t="shared" si="1"/>
+        <v>-84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1234,11 +1334,22 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13">
+        <v>98</v>
+      </c>
+      <c r="O13" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P13" s="8">
+        <f t="shared" si="1"/>
+        <v>-48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1265,11 +1376,22 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="7" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <v>116</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="P14" s="8">
+        <f t="shared" si="1"/>
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -1296,92 +1418,130 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="7" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <v>89</v>
+      </c>
+      <c r="O15" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="P15" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="Q15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L16" s="2"/>
+      <c r="M16" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="N16">
+        <v>24</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P16" s="8">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="Q16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="I17" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="N17">
+        <v>5</v>
+      </c>
+      <c r="O17" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P17" s="8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="Q17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>25</v>
@@ -1391,84 +1551,124 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M18" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P18" s="8">
+        <f t="shared" si="1"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M19" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="N19">
+        <v>25</v>
+      </c>
+      <c r="O19" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P19" s="8">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="Q19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M20" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="N20">
+        <f>100-15</f>
+        <v>85</v>
+      </c>
+      <c r="O20" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="Q20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>97</v>
@@ -1484,22 +1684,33 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M21" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="N21">
+        <v>95</v>
+      </c>
+      <c r="O21" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="3">
-        <v>470</v>
+        <v>99</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>97</v>
@@ -1515,22 +1726,33 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M22" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="N22">
+        <v>95</v>
+      </c>
+      <c r="O22" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="D23" s="3">
+        <v>470</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>97</v>
@@ -1546,22 +1768,33 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M23" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="N23">
+        <v>95</v>
+      </c>
+      <c r="O23" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P23" s="8">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>97</v>
@@ -1577,97 +1810,135 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="N24">
+        <v>95</v>
+      </c>
+      <c r="O24" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P24" s="8">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="1">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="N25">
+        <v>70</v>
+      </c>
+      <c r="O25" s="8">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="P25" s="8">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="Q25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="1">
         <v>27</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B26" s="3">
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3" t="s">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K26" s="3">
         <v>1</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="M26" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="O25" s="7"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="N26">
+        <v>5</v>
+      </c>
+      <c r="O26" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P26" s="8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="Q26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="1">
         <v>28</v>
-      </c>
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>29</v>
       </c>
       <c r="B27" s="3">
         <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>25</v>
@@ -1677,59 +1948,87 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M27" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="O27" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="P27" s="8">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="Q27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O28" s="5"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M28" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="P28" s="8">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="Q28">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1737,414 +2036,530 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="N29">
+        <v>4</v>
+      </c>
+      <c r="O29" s="8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P29" s="8">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="Q29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="1">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F30" s="3" t="s">
+      <c r="N30">
+        <v>8</v>
+      </c>
+      <c r="O30" s="8">
+        <f>B30*50</f>
+        <v>50</v>
+      </c>
+      <c r="P30" s="8">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="Q30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="B32" s="3">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="F32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M32" s="7" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>30</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="N32">
+        <v>175</v>
+      </c>
+      <c r="O32" s="8">
+        <f t="shared" ref="O31:O32" si="2">B32*50</f>
+        <v>400</v>
+      </c>
+      <c r="P32" s="8">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+      <c r="Q32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="1"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="D34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>133</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="D35" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="M35" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="P35" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="1">
+        <v>30</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="1">
+        <v>33</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B57" s="3">
         <v>1</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="G57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B58" s="3">
         <v>2</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="G58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="1">
         <v>16</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B59" s="3">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B60" s="3">
         <v>1</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="G60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B61" s="3">
         <v>1</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+      <c r="G61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="1">
         <v>19</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B62" s="3">
         <v>1</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="1">
         <v>8</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B63" s="3">
         <v>1</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+      <c r="G63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="1">
         <v>7</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B64" s="3">
         <v>4</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="G64" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="1">
         <v>10</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B65" s="3">
         <v>1</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="1">
         <v>11</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B66" s="3">
         <v>1</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="1">
         <v>12</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B67" s="3">
         <v>1</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F67" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="P10:P32">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1" xr:uid="{DEA74A4F-4ECE-BC4A-895C-09E2FFCB5CD3}"/>
-    <hyperlink ref="M25" r:id="rId2" display="https://www.digikey.com/en/products/detail/cui-devices/PT01-D120K2-B103/15903919" xr:uid="{A2EA7ED3-E9ED-8342-BCC5-4EDD693A8C5C}"/>
-    <hyperlink ref="M27" r:id="rId3" display="https://www.digikey.com/en/products/detail/c-k/OS102011MS2QN1/411602" xr:uid="{625C9230-34CB-9E40-BA23-4E6A1F569E2C}"/>
-    <hyperlink ref="M28" r:id="rId4" display="https://www.digikey.com/en/products/detail/diodes-incorporated/AP63300WU-7/10491510" xr:uid="{86763475-26E2-BB47-A9B8-3BE809A0BF34}"/>
-    <hyperlink ref="M29" r:id="rId5" display="https://www.digikey.com/en/products/detail/diodes-incorporated/AP2115M-3-3TRG1/5305574" xr:uid="{57BE4EFE-C2B3-B24A-A34B-5DA95557FE79}"/>
-    <hyperlink ref="M30" r:id="rId6" display="https://www.digikey.com/en/products/detail/metz-connect-usa-inc/09200-71-BDGB00/13536314" xr:uid="{68687878-F205-774B-95FE-DDBC1E6E8524}"/>
-    <hyperlink ref="M17" r:id="rId7" display="https://www.digikey.com/en/products/detail/amphenol-anytek/TC0203620000G/4940295" xr:uid="{D3AF62BA-12E5-3042-935F-0C272FF9F75F}"/>
-    <hyperlink ref="M16" r:id="rId8" display="https://www.digikey.com/en/products/detail/cui-devices/PJ-006A/269296" xr:uid="{C74F3FFC-FEA8-F743-A36D-5C730523B81D}"/>
-    <hyperlink ref="M18" r:id="rId9" display="https://www.digikey.com/en/products/detail/pulse-electronics/BWVS006060454R7ML1/12141053" xr:uid="{E4BAD683-8183-8A43-8AF1-61753E265793}"/>
-    <hyperlink ref="M19" r:id="rId10" display="https://www.digikey.com/en/products/detail/anbon-semiconductor-int-l-limited/BSS138/16708474" xr:uid="{83A4B89F-13C2-DF4C-B9D7-130BA0E99937}"/>
-    <hyperlink ref="M26" r:id="rId11" display="https://www.digikey.com/en/products/detail/omron-electronics-inc-emc-div/B3F-1020/44059" xr:uid="{8D4436A5-E662-8944-893D-08B3F79127C7}"/>
-    <hyperlink ref="M20" r:id="rId12" display="https://www.digikey.com/en/products/detail/yageo/RC0603FR-07158KL/726963" xr:uid="{F316471B-7FA9-6349-AF49-60EAE9CDDC99}"/>
-    <hyperlink ref="M21" r:id="rId13" display="https://www.digikey.com/en/products/detail/yageo/RC0603FR-1330K1L/14286407" xr:uid="{F38CC0AC-6BA5-264A-BD1B-F6A89D7FC838}"/>
-    <hyperlink ref="M22" r:id="rId14" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/WR06X471-JTL/13240608" xr:uid="{CD96E7D4-147E-704F-A952-824B1747C88A}"/>
-    <hyperlink ref="M23" r:id="rId15" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/WR06X332-JTL/13241747" xr:uid="{3366BBE4-0D4E-5A48-8659-D95480597405}"/>
-    <hyperlink ref="M24" r:id="rId16" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/WR06X103-JTL/13239132" xr:uid="{2F1F431A-77F9-5C40-9D11-A9CF4A220D84}"/>
+    <hyperlink ref="G20" r:id="rId1" xr:uid="{DEA74A4F-4ECE-BC4A-895C-09E2FFCB5CD3}"/>
+    <hyperlink ref="M26" r:id="rId2" display="https://www.digikey.com/en/products/detail/cui-devices/PT01-D120K2-B103/15903919" xr:uid="{A2EA7ED3-E9ED-8342-BCC5-4EDD693A8C5C}"/>
+    <hyperlink ref="M28" r:id="rId3" display="https://www.digikey.com/en/products/detail/c-k/OS102011MS2QN1/411602" xr:uid="{625C9230-34CB-9E40-BA23-4E6A1F569E2C}"/>
+    <hyperlink ref="M29" r:id="rId4" display="https://www.digikey.com/en/products/detail/diodes-incorporated/AP63300WU-7/10491510" xr:uid="{86763475-26E2-BB47-A9B8-3BE809A0BF34}"/>
+    <hyperlink ref="M30" r:id="rId5" display="https://www.digikey.com/en/products/detail/diodes-incorporated/AP2115M-3-3TRG1/5305574" xr:uid="{57BE4EFE-C2B3-B24A-A34B-5DA95557FE79}"/>
+    <hyperlink ref="M32" r:id="rId6" display="https://www.digikey.com/en/products/detail/metz-connect-usa-inc/09200-71-BDGB00/13536314" xr:uid="{68687878-F205-774B-95FE-DDBC1E6E8524}"/>
+    <hyperlink ref="M18" r:id="rId7" display="https://www.digikey.com/en/products/detail/amphenol-anytek/TC0203620000G/4940295" xr:uid="{D3AF62BA-12E5-3042-935F-0C272FF9F75F}"/>
+    <hyperlink ref="M17" r:id="rId8" display="https://www.digikey.com/en/products/detail/cui-devices/PJ-006A/269296" xr:uid="{C74F3FFC-FEA8-F743-A36D-5C730523B81D}"/>
+    <hyperlink ref="M19" r:id="rId9" display="https://www.digikey.com/en/products/detail/pulse-electronics/BWVS006060454R7ML1/12141053" xr:uid="{E4BAD683-8183-8A43-8AF1-61753E265793}"/>
+    <hyperlink ref="M20" r:id="rId10" display="https://www.digikey.com/en/products/detail/anbon-semiconductor-int-l-limited/BSS138/16708474" xr:uid="{83A4B89F-13C2-DF4C-B9D7-130BA0E99937}"/>
+    <hyperlink ref="M27" r:id="rId11" display="https://www.digikey.com/en/products/detail/omron-electronics-inc-emc-div/B3F-1020/44059" xr:uid="{8D4436A5-E662-8944-893D-08B3F79127C7}"/>
+    <hyperlink ref="M21" r:id="rId12" display="https://www.digikey.com/en/products/detail/yageo/RC0603FR-07158KL/726963" xr:uid="{F316471B-7FA9-6349-AF49-60EAE9CDDC99}"/>
+    <hyperlink ref="M22" r:id="rId13" display="https://www.digikey.com/en/products/detail/yageo/RC0603FR-1330K1L/14286407" xr:uid="{F38CC0AC-6BA5-264A-BD1B-F6A89D7FC838}"/>
+    <hyperlink ref="M23" r:id="rId14" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/WR06X471-JTL/13240608" xr:uid="{CD96E7D4-147E-704F-A952-824B1747C88A}"/>
+    <hyperlink ref="M24" r:id="rId15" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/WR06X332-JTL/13241747" xr:uid="{3366BBE4-0D4E-5A48-8659-D95480597405}"/>
+    <hyperlink ref="M25" r:id="rId16" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/WR06X103-JTL/13239132" xr:uid="{2F1F431A-77F9-5C40-9D11-A9CF4A220D84}"/>
     <hyperlink ref="M10" r:id="rId17" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05A104KA5NNNC/3886701" xr:uid="{2C82E486-5F82-AD41-AC01-8E80A5A3FE49}"/>
     <hyperlink ref="M11" r:id="rId18" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21X226MRQNNNE/3886860" xr:uid="{D0C83157-75A8-B341-93C4-DFE2463615E9}"/>
     <hyperlink ref="M12" r:id="rId19" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A106KOQNNNE/3886754" xr:uid="{5D6F156C-4704-B443-9D06-ADB526B84CDA}"/>
     <hyperlink ref="M13" r:id="rId20" display="https://www.digikey.com/en/products/detail/walsin-technology-corporation/0603N470J500CT/9355025" xr:uid="{70E9D692-A8D8-0549-BD3B-AAE76EF3077D}"/>
     <hyperlink ref="M14" r:id="rId21" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10A475KQ8NNNC/3886703" xr:uid="{A5F56DCE-57F6-E944-9EB2-CA67EDA22A50}"/>
     <hyperlink ref="M15" r:id="rId22" display="https://www.digikey.com/en/products/detail/harvatek-corporation/B1911USD-20D000114U1930/15519991" xr:uid="{C748F7B0-1CE3-5B44-A0FA-9255E70DAEEB}"/>
+    <hyperlink ref="M33" r:id="rId23" display="https://www.amazon.com/gp/product/B0817JG3XN/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1" xr:uid="{83DE12D9-5AEF-9240-BE0F-E2D2FF216120}"/>
+    <hyperlink ref="M34" r:id="rId24" display="https://www.amazon.com/gp/product/B07CGGSDWF/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1" xr:uid="{E38711A0-DA95-2F44-B6BA-D94E4311CAF5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>